<commit_message>
Add Version info from emeScheme.xls
Version info is added to:

* to DESCRIPTION file
* all emeScheme files
* all exported file formats, including xml
* test is added yto verify the versions in the DESCRIPTION file and the emeScheme.xlsx are in sync
</commit_message>
<xml_diff>
--- a/inst/emeScheme.xlsx
+++ b/inst/emeScheme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rainer/Documents/Projects/DataManagementAndStrategy/emeScheme/inst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70611AA0-0D15-6743-BC51-5DE7094BFC28}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485B5043-89DA-5445-B174-79354C0E5257}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="28360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="189">
   <si>
     <t>propertySet</t>
   </si>
@@ -1311,6 +1311,9 @@
   </si>
   <si>
     <t>presens Optode, microscopy</t>
+  </si>
+  <si>
+    <t>DATA_v0.9.5</t>
   </si>
 </sst>
 </file>
@@ -3432,7 +3435,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3446,7 +3449,7 @@
     <col min="7" max="7" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3466,10 +3469,10 @@
         <v>8</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
         <v>12</v>
       </c>
@@ -3704,7 +3707,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A15" s="81"/>
       <c r="B15" s="83" t="s">
         <v>24</v>
@@ -3722,7 +3725,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Note that can enter an item not in the provided list. This is OK so long as you really intended this. Ignore the Invalid entry message you then get" sqref="G12" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"treatment,single trophic level,multiple trophic level,…"</formula1>
     </dataValidation>
@@ -3744,7 +3747,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>